<commit_message>
random forest and slight corrections
</commit_message>
<xml_diff>
--- a/data/databasecsv.xlsx
+++ b/data/databasecsv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximeducotterd/Desktop/finalcapstone/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximeducotterd/Desktop/DSAP_intercantonal_dynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5034745C-6A1D-294E-95F3-66303C39D988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC4FF5E-0EB0-3B43-96B8-45AA2F3A3C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{84DBC18D-2D30-E647-B564-5004DFEC53A4}"/>
   </bookViews>
@@ -351,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -394,13 +394,12 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2033,13 +2032,13 @@
   </sheetPr>
   <dimension ref="A1:AL286"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="107" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="16.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="16.1640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.1640625" style="6" customWidth="1"/>

</xml_diff>

<commit_message>
Make all the script testable and create test files
</commit_message>
<xml_diff>
--- a/data/databasecsv.xlsx
+++ b/data/databasecsv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximeducotterd/Desktop/DSAP_intercantonal_dynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC4FF5E-0EB0-3B43-96B8-45AA2F3A3C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F103EA7-44FF-9840-930C-B0FBBF66D429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{84DBC18D-2D30-E647-B564-5004DFEC53A4}"/>
   </bookViews>
@@ -2032,8 +2032,8 @@
   </sheetPr>
   <dimension ref="A1:AL286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2291,8 +2291,8 @@
         <v>0</v>
       </c>
       <c r="AG2" s="14">
-        <f>LN(1+AF2)</f>
-        <v>0</v>
+        <f>AG8</f>
+        <v>0.10337295958495014</v>
       </c>
       <c r="AH2" s="14">
         <f>(AF2-AVERAGE($AF$2:$AF$261))/STDEV($AF$2:$AF$261)</f>

</xml_diff>